<commit_message>
adding nxt gen matrix modeling
</commit_message>
<xml_diff>
--- a/ParameterValues.xlsx
+++ b/ParameterValues.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gitrepos\MetaDisease\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDD69CE2-D24F-4135-84C6-1949F2F078ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{756C7DAA-6891-462F-9054-C5522437247F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11895" yWindow="0" windowWidth="12210" windowHeight="12885" xr2:uid="{FA5DE44C-DA56-4EB2-992C-9D9CEF12A138}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{FA5DE44C-DA56-4EB2-992C-9D9CEF12A138}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -536,7 +536,7 @@
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
made R0sp = beta_ss/b
</commit_message>
<xml_diff>
--- a/ParameterValues.xlsx
+++ b/ParameterValues.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gitrepos\MetaDisease\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{756C7DAA-6891-462F-9054-C5522437247F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F677EED6-4D1E-454D-8F80-3C5581347567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{FA5DE44C-DA56-4EB2-992C-9D9CEF12A138}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="1" xr2:uid="{FA5DE44C-DA56-4EB2-992C-9D9CEF12A138}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="PerDay" sheetId="1" r:id="rId1"/>
+    <sheet name="PerSeason" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="39">
   <si>
     <t>Species</t>
   </si>
@@ -535,8 +536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9D18438-9C45-4FFD-AEEC-D117EBEF019E}">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -695,8 +696,8 @@
         <v>15</v>
       </c>
       <c r="G6">
-        <f>1 - ((4+2+1+4)/(15+4+4+11))^((1/33))</f>
-        <v>3.3617844334099534E-2</v>
+        <f>1 - ((4+2+1+4)/(15+4+4+11))^((1/365))</f>
+        <v>3.0869112829463585E-3</v>
       </c>
       <c r="H6" t="s">
         <v>22</v>
@@ -783,4 +784,253 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57BE2E86-A394-4241-BDAC-A29C04F4FD59}">
+  <dimension ref="A1:K17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="46.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="35.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <f>1-(0.11^(1/90))</f>
+        <v>2.4226975825790698E-2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2">
+        <v>0.83</v>
+      </c>
+      <c r="J2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3">
+        <v>0.62</v>
+      </c>
+      <c r="K3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="K4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <f>1-(0.77^(1/90))</f>
+        <v>2.8998402520405975E-3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <f>1-(((0.37+0.17)/2)^(1/90))</f>
+        <v>1.4442835016211797E-2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6">
+        <f>1 - ((4+2+1+4)/(15+4+4+11))^((1/90))</f>
+        <v>1.2460223282640404E-2</v>
+      </c>
+      <c r="H6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6">
+        <v>0.12</v>
+      </c>
+      <c r="K6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <f>1-(0.0263^(1/90))</f>
+        <v>3.9618130288291642E-2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7">
+        <v>0.64</v>
+      </c>
+      <c r="K7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
found parameters for prevalence. just need beta
</commit_message>
<xml_diff>
--- a/ParameterValues.xlsx
+++ b/ParameterValues.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gitrepos\MetaDisease\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F677EED6-4D1E-454D-8F80-3C5581347567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA14D0D-D9DE-4630-918E-8E1276F620B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="1" xr2:uid="{FA5DE44C-DA56-4EB2-992C-9D9CEF12A138}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{FA5DE44C-DA56-4EB2-992C-9D9CEF12A138}"/>
   </bookViews>
   <sheets>
     <sheet name="PerDay" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="44">
   <si>
     <t>Species</t>
   </si>
@@ -154,6 +154,21 @@
   </si>
   <si>
     <t>Colonization*(1/N)</t>
+  </si>
+  <si>
+    <t>disease induced mortality</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>McMahon 2023</t>
+  </si>
+  <si>
+    <t>Carey et al 2006</t>
+  </si>
+  <si>
+    <t>Padgett Flohr 2008</t>
   </si>
 </sst>
 </file>
@@ -534,9 +549,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9D18438-9C45-4FFD-AEEC-D117EBEF019E}">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -550,9 +565,11 @@
     <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="32.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="32.5703125" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -586,8 +603,14 @@
       <c r="K1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -613,8 +636,15 @@
       <c r="K2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2">
+        <f>-LOG(1-0.13)/14</f>
+        <v>4.3200533843843914E-3</v>
+      </c>
+      <c r="M2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -636,8 +666,11 @@
       <c r="K3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -659,8 +692,11 @@
       <c r="K4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -680,8 +716,15 @@
       <c r="I5" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5">
+        <f>-LOG(0.5)/42</f>
+        <v>7.1673808491424093E-3</v>
+      </c>
+      <c r="M5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -708,8 +751,14 @@
       <c r="K6" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -732,43 +781,49 @@
       <c r="K7" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -788,10 +843,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57BE2E86-A394-4241-BDAC-A29C04F4FD59}">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -802,9 +857,11 @@
     <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="35.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -838,8 +895,14 @@
       <c r="K1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -865,8 +928,14 @@
       <c r="K2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2">
+        <v>0.13</v>
+      </c>
+      <c r="M2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -888,8 +957,11 @@
       <c r="K3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -911,8 +983,11 @@
       <c r="K4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -932,8 +1007,14 @@
       <c r="I5" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -960,8 +1041,14 @@
       <c r="K6" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -984,43 +1071,49 @@
       <c r="K7" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
made single script for 2 and 5 patch systems
</commit_message>
<xml_diff>
--- a/ParameterValues.xlsx
+++ b/ParameterValues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gitrepos\MetaDisease\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA14D0D-D9DE-4630-918E-8E1276F620B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C53E4B76-0924-4EC4-8336-8EE69B43DBFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{FA5DE44C-DA56-4EB2-992C-9D9CEF12A138}"/>
   </bookViews>
@@ -551,7 +551,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9D18438-9C45-4FFD-AEEC-D117EBEF019E}">
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>

</xml_diff>